<commit_message>
Failing test for customer addTransaction method
</commit_message>
<xml_diff>
--- a/Bank Challenge Domain Model.xlsx
+++ b/Bank Challenge Domain Model.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -127,6 +127,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -148,6 +149,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -221,15 +223,15 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Write readme, final comments
</commit_message>
<xml_diff>
--- a/Bank Challenge Domain Model.xlsx
+++ b/Bank Challenge Domain Model.xlsx
@@ -222,11 +222,11 @@
   </sheetPr>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H32" activeCellId="0" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.34"/>

</xml_diff>